<commit_message>
£TRLS Cash Per Share (CPS) metric
</commit_message>
<xml_diff>
--- a/£TRLS.xlsx
+++ b/£TRLS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371263E2-E877-4E50-A850-E4EA1C7B4FD3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EDE517-5C42-47AE-925A-F3D3445B4820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18915" xr2:uid="{22FE4D90-709B-430A-8239-4013C6F51091}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22FE4D90-709B-430A-8239-4013C6F51091}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -156,9 +165,6 @@
     <t>P/S</t>
   </si>
   <si>
-    <t>P/E</t>
-  </si>
-  <si>
     <t>Investor Presentations</t>
   </si>
   <si>
@@ -334,6 +340,9 @@
   </si>
   <si>
     <t>Initial demonstration project will be offered via New York Medicaid health plan with more than 1.8m members</t>
+  </si>
+  <si>
+    <t>CPS</t>
   </si>
 </sst>
 </file>
@@ -614,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -750,8 +759,6 @@
     <xf numFmtId="15" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -759,12 +766,6 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -774,8 +775,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,6 +799,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1192,7 +1203,7 @@
   <dimension ref="A2:AB35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1207,7 +1218,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2"/>
     </row>
@@ -1217,37 +1228,37 @@
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="84"/>
-      <c r="G5" s="82" t="s">
+      <c r="C5" s="79"/>
+      <c r="D5" s="80"/>
+      <c r="G5" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="83"/>
-      <c r="P5" s="83"/>
-      <c r="Q5" s="83"/>
-      <c r="R5" s="84"/>
-      <c r="T5" s="82" t="s">
-        <v>60</v>
-      </c>
-      <c r="U5" s="83"/>
-      <c r="V5" s="83"/>
-      <c r="W5" s="83"/>
-      <c r="X5" s="84"/>
-      <c r="Z5" s="82" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA5" s="83"/>
-      <c r="AB5" s="84"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="80"/>
+      <c r="T5" s="78" t="s">
+        <v>59</v>
+      </c>
+      <c r="U5" s="79"/>
+      <c r="V5" s="79"/>
+      <c r="W5" s="79"/>
+      <c r="X5" s="80"/>
+      <c r="Z5" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA5" s="79"/>
+      <c r="AB5" s="80"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
@@ -1258,19 +1269,19 @@
       </c>
       <c r="D6" s="6"/>
       <c r="G6" s="18"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="75"/>
-      <c r="Q6" s="75"/>
-      <c r="R6" s="76"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="13"/>
       <c r="T6" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U6" s="12"/>
       <c r="V6" s="12"/>
@@ -1279,10 +1290,10 @@
       <c r="Z6" s="70">
         <v>44835</v>
       </c>
-      <c r="AA6" s="87" t="s">
+      <c r="AA6" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="AB6" s="88"/>
+      <c r="AB6" s="82"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
@@ -1296,25 +1307,25 @@
         <v>FY21</v>
       </c>
       <c r="G7" s="18"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="75"/>
-      <c r="M7" s="75"/>
-      <c r="N7" s="75"/>
-      <c r="O7" s="75"/>
-      <c r="P7" s="75"/>
-      <c r="Q7" s="75"/>
-      <c r="R7" s="76"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="13"/>
       <c r="T7" s="33"/>
       <c r="U7" s="12"/>
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
       <c r="X7" s="13"/>
       <c r="Z7" s="22"/>
-      <c r="AA7" s="89"/>
-      <c r="AB7" s="90"/>
+      <c r="AA7" s="83"/>
+      <c r="AB7" s="84"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
@@ -1325,22 +1336,22 @@
         <v>8.5604999999999993</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="G8" s="77">
+      <c r="G8" s="75">
         <v>44958</v>
       </c>
-      <c r="H8" s="79" t="s">
-        <v>93</v>
-      </c>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="75"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="75"/>
-      <c r="Q8" s="75"/>
-      <c r="R8" s="76"/>
+      <c r="H8" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="13"/>
       <c r="T8" s="33"/>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
@@ -1360,19 +1371,19 @@
         <v>FY21</v>
       </c>
       <c r="G9" s="18"/>
-      <c r="H9" s="78" t="s">
-        <v>94</v>
-      </c>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="76"/>
+      <c r="H9" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="13"/>
       <c r="T9" s="33"/>
       <c r="U9" s="12"/>
       <c r="V9" s="12"/>
@@ -1391,17 +1402,17 @@
         <v>FY21</v>
       </c>
       <c r="G10" s="18"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="75"/>
-      <c r="P10" s="75"/>
-      <c r="Q10" s="75"/>
-      <c r="R10" s="76"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="13"/>
       <c r="T10" s="33"/>
       <c r="U10" s="12"/>
       <c r="V10" s="12"/>
@@ -1420,11 +1431,11 @@
         <f t="shared" si="0"/>
         <v>FY21</v>
       </c>
-      <c r="G11" s="77">
+      <c r="G11" s="75">
         <v>44958</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
@@ -1452,8 +1463,8 @@
       </c>
       <c r="D12" s="7"/>
       <c r="G12" s="18"/>
-      <c r="H12" s="78" t="s">
-        <v>92</v>
+      <c r="H12" s="76" t="s">
+        <v>91</v>
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
@@ -1473,7 +1484,7 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="B13" s="67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="65">
         <v>0.88</v>
@@ -1521,11 +1532,11 @@
       <c r="X14" s="16"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="84"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="80"/>
       <c r="G15" s="18"/>
       <c r="H15" s="19" t="s">
         <v>15</v>
@@ -1548,10 +1559,10 @@
       <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="80" t="s">
+      <c r="C16" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="81"/>
+      <c r="D16" s="92"/>
       <c r="G16" s="18"/>
       <c r="H16" s="19" t="s">
         <v>16</v>
@@ -1572,10 +1583,10 @@
       <c r="B17" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="80" t="s">
+      <c r="C17" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="81"/>
+      <c r="D17" s="92"/>
       <c r="G17" s="18"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -1596,18 +1607,18 @@
       <c r="B18" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="80" t="s">
+      <c r="C18" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="81"/>
+      <c r="D18" s="92"/>
       <c r="E18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -1624,10 +1635,10 @@
       <c r="B19" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="96"/>
+      <c r="D19" s="90"/>
       <c r="G19" s="18"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -1646,7 +1657,7 @@
         <v>44344</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -1674,11 +1685,11 @@
       <c r="R21" s="13"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="83"/>
-      <c r="D22" s="84"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="80"/>
       <c r="G22" s="18"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -1696,10 +1707,10 @@
       <c r="B23" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="80" t="s">
+      <c r="C23" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="81"/>
+      <c r="D23" s="92"/>
       <c r="G23" s="18"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -1717,10 +1728,10 @@
       <c r="B24" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="80">
+      <c r="C24" s="91">
         <v>2020</v>
       </c>
-      <c r="D24" s="81"/>
+      <c r="D24" s="92"/>
       <c r="G24" s="18"/>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -1736,8 +1747,8 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="18"/>
-      <c r="C25" s="91"/>
-      <c r="D25" s="92"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="86"/>
       <c r="G25" s="18"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -1753,8 +1764,8 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B26" s="18"/>
-      <c r="C26" s="91"/>
-      <c r="D26" s="92"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="86"/>
       <c r="G26" s="18"/>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
@@ -1770,8 +1781,8 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B27" s="18"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="92"/>
+      <c r="C27" s="85"/>
+      <c r="D27" s="86"/>
       <c r="G27" s="20"/>
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
@@ -1790,7 +1801,7 @@
         <v>30</v>
       </c>
       <c r="C28" s="68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" s="13"/>
     </row>
@@ -1798,48 +1809,57 @@
       <c r="B29" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="89" t="s">
+      <c r="C29" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="90"/>
+      <c r="D29" s="84"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B32" s="82" t="s">
+      <c r="B32" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="83"/>
-      <c r="D32" s="84"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="80"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="93">
+      <c r="C33" s="87">
         <f>C6/'Financial Model'!P45</f>
         <v>0.2426858309236265</v>
       </c>
-      <c r="D33" s="94"/>
+      <c r="D33" s="88"/>
       <c r="G33" s="31"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="93">
+      <c r="C34" s="87">
         <f>C8/'Financial Model'!P4</f>
         <v>0.34241999999999995</v>
       </c>
-      <c r="D34" s="94"/>
+      <c r="D34" s="88"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="85"/>
-      <c r="D35" s="86"/>
+        <v>94</v>
+      </c>
+      <c r="C35" s="93">
+        <f>C11/C7</f>
+        <v>0.21369901290812454</v>
+      </c>
+      <c r="D35" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="G5:R5"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="Z5:AB5"/>
     <mergeCell ref="AA6:AB6"/>
@@ -1856,12 +1876,6 @@
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="G5:R5"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C29:D29" r:id="rId1" display="Link" xr:uid="{03F0450A-3559-4A6F-9878-BC2701BC0DAB}"/>
@@ -1901,40 +1915,40 @@
   <sheetData>
     <row r="1" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="24" t="s">
+      <c r="P1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="P1" s="23" t="s">
+      <c r="Q1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="R1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="S1" s="23" t="s">
         <v>46</v>
-      </c>
-      <c r="S1" s="23" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="27" customFormat="1" x14ac:dyDescent="0.2">
@@ -1967,7 +1981,7 @@
     </row>
     <row r="4" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="51"/>
       <c r="D4" s="36"/>
@@ -1982,7 +1996,7 @@
     </row>
     <row r="5" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="52"/>
       <c r="D5" s="37"/>
@@ -1997,7 +2011,7 @@
     </row>
     <row r="6" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="51"/>
       <c r="D6" s="36"/>
@@ -2014,7 +2028,7 @@
     </row>
     <row r="7" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="52"/>
       <c r="D7" s="37"/>
@@ -2029,7 +2043,7 @@
     </row>
     <row r="8" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="51"/>
       <c r="D8" s="36"/>
@@ -2047,7 +2061,7 @@
     <row r="9" spans="1:19" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="38"/>
       <c r="B9" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="53"/>
       <c r="D9" s="40"/>
@@ -2063,7 +2077,7 @@
     <row r="10" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="41"/>
       <c r="B10" s="42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="54"/>
       <c r="D10" s="43"/>
@@ -2079,7 +2093,7 @@
     <row r="11" spans="1:19" s="45" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="44"/>
       <c r="B11" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="55"/>
       <c r="D11" s="46"/>
@@ -2096,7 +2110,7 @@
     </row>
     <row r="12" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="52"/>
       <c r="D12" s="37"/>
@@ -2111,7 +2125,7 @@
     </row>
     <row r="13" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B13" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="52"/>
       <c r="D13" s="37"/>
@@ -2126,7 +2140,7 @@
     </row>
     <row r="14" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="52"/>
       <c r="D14" s="37"/>
@@ -2143,7 +2157,7 @@
     </row>
     <row r="15" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="52"/>
       <c r="D15" s="37"/>
@@ -2158,7 +2172,7 @@
     </row>
     <row r="16" spans="1:19" s="32" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="51"/>
       <c r="D16" s="36"/>
@@ -2175,7 +2189,7 @@
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O17" s="63">
         <f>O16/O18</f>
@@ -2199,7 +2213,7 @@
     </row>
     <row r="20" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="57"/>
       <c r="D20" s="30"/>
@@ -2210,15 +2224,15 @@
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O23" s="61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P23" s="60">
         <f>P6/P4</f>
@@ -2227,10 +2241,10 @@
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O24" s="61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P24" s="60">
         <f>P8/P4</f>
@@ -2239,10 +2253,10 @@
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O25" s="61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P25" s="60">
         <f>P16/P4</f>
@@ -2251,10 +2265,10 @@
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O26" s="61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P26" s="60">
         <f>P17/P16</f>
@@ -2263,13 +2277,13 @@
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B29" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O29" s="52"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="52">
         <v>32</v>
@@ -2287,7 +2301,7 @@
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="52">
         <v>2214</v>
@@ -2305,7 +2319,7 @@
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32" s="52">
         <v>0</v>
@@ -2323,7 +2337,7 @@
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="52">
         <f>C30+C31+C32</f>
@@ -2344,7 +2358,7 @@
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="52">
         <v>319</v>
@@ -2382,7 +2396,7 @@
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="52">
         <f>C33+SUM(C34:C35)</f>
@@ -2408,7 +2422,7 @@
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C38" s="52">
         <v>1032</v>
@@ -2426,7 +2440,7 @@
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" s="52">
         <f>C38</f>
@@ -2451,7 +2465,7 @@
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C41" s="52">
         <v>41224</v>
@@ -2469,7 +2483,7 @@
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" s="52">
         <f>C41+C39</f>
@@ -2490,7 +2504,7 @@
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O44" s="52">
         <f>O36-O39</f>
@@ -2503,7 +2517,7 @@
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O45" s="56">
         <f>O44/O18</f>
@@ -2575,13 +2589,13 @@
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C51" s="61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D51" s="72" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P51" s="60">
         <f>P49/O49-1</f>
@@ -2590,20 +2604,20 @@
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C52" s="61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D52" s="25">
         <f>D49/C49-1</f>
         <v>-0.19422539114660753</v>
       </c>
       <c r="O52" s="61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P52" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>